<commit_message>
QLBM - Send email to all
</commit_message>
<xml_diff>
--- a/Code/QLBM/QuanLyBoMon/bin/Debug/LichGiangDay/GiangVien_ĐỖ-THỊ-HẠNH_LichGiangDay.xlsx
+++ b/Code/QLBM/QuanLyBoMon/bin/Debug/LichGiangDay/GiangVien_ĐỖ-THỊ-HẠNH_LichGiangDay.xlsx
@@ -35,7 +35,7 @@
     <t>Năm học:</t>
   </si>
   <si>
-    <t>2015</t>
+    <t>2015-2016</t>
   </si>
   <si>
     <t>Tên Lớp</t>
@@ -104,10 +104,10 @@
     <t/>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
     <t>YHCT2012</t>
+  </si>
+  <si>
+    <t>CNXH</t>
   </si>
   <si>
     <t>22/02/2016-04/06/2016</t>
@@ -723,9 +723,7 @@
       <c r="I7" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="J7" s="13" t="s">
-        <v>27</v>
-      </c>
+      <c r="J7" s="13"/>
       <c r="K7" s="13" t="s">
         <v>26</v>
       </c>
@@ -738,84 +736,78 @@
       <c r="N7" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="O7" s="13" t="s">
-        <v>27</v>
-      </c>
+      <c r="O7" s="13"/>
       <c r="P7" s="13" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="8" ht="12" s="9" customFormat="1">
       <c r="A8" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>22</v>
-      </c>
       <c r="C8" s="13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="H8" s="13" t="s">
         <v>26</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="J8" s="13" t="s">
-        <v>27</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="J8" s="13"/>
       <c r="K8" s="13" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="L8" s="13" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="M8" s="13" t="s">
         <v>26</v>
       </c>
       <c r="N8" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="O8" s="13" t="s">
-        <v>27</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="O8" s="13"/>
       <c r="P8" s="13" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" ht="12" s="9" customFormat="1">
       <c r="A9" s="13" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B9" s="13" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>31</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="H9" s="13" t="s">
         <v>26</v>
@@ -823,14 +815,12 @@
       <c r="I9" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="J9" s="13" t="s">
-        <v>27</v>
-      </c>
+      <c r="J9" s="13"/>
       <c r="K9" s="13" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="L9" s="13" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="M9" s="13" t="s">
         <v>26</v>
@@ -838,30 +828,56 @@
       <c r="N9" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="O9" s="13" t="s">
-        <v>27</v>
-      </c>
+      <c r="O9" s="13"/>
       <c r="P9" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" ht="12" s="9" customFormat="1">
+      <c r="A10" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="13" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" ht="12" s="9" customFormat="1">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
+      <c r="G10" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="L10" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="M10" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="N10" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="11" ht="12" s="9" customFormat="1">
       <c r="A11" s="10"/>
@@ -3136,6 +3152,7 @@
     <mergeCell ref="D1:M2"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="L4:M4"/>
+    <mergeCell ref="A8:A9"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" verticalDpi="300"/>

</xml_diff>